<commit_message>
them báo cáo đồ án và sửa xong app giáo viên
</commit_message>
<xml_diff>
--- a/ApiExpress/public/upload/importStudent.xlsx
+++ b/ApiExpress/public/upload/importStudent.xlsx
@@ -317,122 +317,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="14.5703125"/>
-    <col min="2" max="2" customWidth="1" width="13.140625"/>
-    <col min="3" max="3" customWidth="1" width="13.5703125"/>
-    <col min="4" max="4" customWidth="1" width="9.7109375"/>
-    <col min="5" max="5" customWidth="1" width="16.7109375"/>
-    <col min="6" max="6" customWidth="1" width="18.28515625"/>
-    <col min="8" max="8" customWidth="1" width="16.85546875"/>
+    <col min="1" max="1" customWidth="1" width="13.5703125"/>
+    <col min="2" max="2" customWidth="1" width="14.5703125"/>
+    <col min="3" max="3" customWidth="1" width="13.140625"/>
+    <col min="4" max="4" customWidth="1" width="13.5703125"/>
+    <col min="5" max="5" customWidth="1" width="9.7109375"/>
+    <col min="6" max="6" customWidth="1" width="16.7109375"/>
+    <col min="7" max="7" customWidth="1" width="30.85546875"/>
+    <col min="9" max="9" customWidth="1" width="16.85546875"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>name</v>
+        <v>first_name</v>
       </c>
       <c r="B1" t="str">
+        <v>last_name</v>
+      </c>
+      <c r="C1" t="str">
         <v>mssv</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>phone</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>birthday</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>address</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>email</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>sex</v>
       </c>
     </row>
-    <row r="2" ht="75.75" customHeight="1">
+    <row r="2" ht="31.5" customHeight="1">
       <c r="A2" t="str">
-        <v>Lê Văn Hải</v>
-      </c>
-      <c r="B2">
-        <v>20170956</v>
+        <v>Trần Văn</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Khang</v>
       </c>
       <c r="C2">
-        <v>987564444</v>
-      </c>
-      <c r="D2" s="1">
-        <v>36466</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Bắc giang</v>
+        <v>20140956</v>
+      </c>
+      <c r="D2">
+        <v>987884444</v>
+      </c>
+      <c r="E2" s="1">
+        <v>35371</v>
       </c>
       <c r="F2" t="str">
-        <v>hailv@gmail.com</v>
+        <v>Hà Giang</v>
       </c>
       <c r="G2" t="str">
+        <v>khangtv20140956@gmail.com</v>
+      </c>
+      <c r="H2" t="str">
         <v>nam</v>
       </c>
     </row>
-    <row r="3" ht="75" customHeight="1">
-      <c r="A3" t="str">
-        <v>Trần Văn Nam</v>
-      </c>
-      <c r="B3">
-        <v>20164987</v>
-      </c>
-      <c r="C3">
-        <v>987987457</v>
-      </c>
-      <c r="D3" s="1">
-        <v>35465</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Nghệ An</v>
-      </c>
-      <c r="F3" t="str">
-        <v>namtv@gmail.com</v>
-      </c>
-      <c r="G3" t="str">
-        <v>nam</v>
-      </c>
-    </row>
-    <row r="4" ht="75" customHeight="1">
-      <c r="A4" t="str">
-        <v>Trần Đức Thọ</v>
-      </c>
-      <c r="B4">
-        <v>20174977</v>
-      </c>
-      <c r="C4">
-        <v>987977457</v>
-      </c>
-      <c r="D4" s="1">
-        <v>35830</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Nghệ An</v>
-      </c>
-      <c r="F4" t="str">
-        <v>thotd@gmail.com</v>
-      </c>
-      <c r="G4" t="str">
-        <v>nam</v>
-      </c>
-    </row>
+    <row r="3" ht="75" customHeight="1"/>
+    <row r="4" ht="75" customHeight="1"/>
     <row r="6"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>